<commit_message>
DImensioning and operation of original case
The model is including a case study with around 25 buidlings that is
first ran for dimensioning optim. and then taking into account the
results of this, for operation optimization. It refers to a case with no
bidding
</commit_message>
<xml_diff>
--- a/z.For the new model/MODELS.xlsx
+++ b/z.For the new model/MODELS.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="90" windowWidth="12435" windowHeight="6465" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="90" windowWidth="12435" windowHeight="6465"/>
   </bookViews>
   <sheets>
     <sheet name="Option5" sheetId="1" r:id="rId1"/>
@@ -332,9 +332,6 @@
     <t>Income_via_exports</t>
   </si>
   <si>
-    <t>sum(x | x = 'Elec', Electricity_feedin_price_renewables * sum(t, Exported_energy_renewable(t,x)) + Electricity_feedin_price_nonrenewables * sum(t, Exported_energy_nonrenewable(t,x))) + sum(t, pr_P_W_TRLplus(t)*P_W_TRLplus(t,'Elec'))/168 +  sum(t, pr_P_D_TRLplus(t)*P_D_TRLplus(t,'Elec'))/4 + pr_E_W_TRLplus*sum(t,a_TRLplus(t)*E_W_TRLplus(t,'Elec'))*4/4 +  pr_E_D_TRLplus*sum(t,a_TRLplus(t)*E_D_TRLplus(t,'Elec'))*4/4 + pr_E_LM_TRLplus*sum(t,a_TRLplus(t)*E_LM_TRLplus(t,'Elec'))*4/4</t>
-  </si>
-  <si>
     <t>Total_cost</t>
   </si>
   <si>
@@ -377,6 +374,13 @@
   <si>
     <t>sum(x | x = 'Elec', Electricity_feedin_price_renewables * sum(t, Exported_energy_renewable(t,x)) + Electricity_feedin_price_nonrenewables * sum(t, Exported_energy_nonrenewable(t,x))) + 
 sum(t, pr_P_W_TRLplus(t)*P_W_TRLplus(t,'Elec'))/168 +  sum(t, pr_P_D_TRLplus(t)*P_D_TRLplus(t,'Elec'))/4 + pr_E_W_TRLplus*sum(t,aw_TRLplus(t)*E_W_TRLplus(t,'Elec'))*4/4 +  pr_E_D_TRLplus*sum(t,ad_TRLplus(t)*E_D_TRLplus(t,'Elec'))*4/4 + pr_E_LM_TRLplus*sum(t,alm_TRLplus(t)*E_LM_TRLplus(t,'Elec'))*4/4</t>
+  </si>
+  <si>
+    <t>sum(x | x = 'Elec', Electricity_feedin_price_renewables * sum(t, Exported_energy_renewable(t,x)) + 
+Electricity_feedin_price_nonrenewables * sum(t, Exported_energy_nonrenewable(t,x))) + 
+sum(t, pr_P_W_TRLplus(t)*P_W_TRLplus(t,'Elec'))/168 +  sum(t, pr_P_D_TRLplus(t)*P_D_TRLplus(t,'Elec'))/4 + 
+pr_E_W_TRLplus*sum(t,a_TRLplus(t)*E_W_TRLplus(t,'Elec'))*4/4 +  pr_E_D_TRLplus*sum(t,a_TRLplus(t)*E_D_TRLplus(t,'Elec'))*4/4 + 
+pr_E_LM_TRLplus*sum(t,a_TRLplus(t)*E_LM_TRLplus(t,'Elec'))*4/4</t>
   </si>
 </sst>
 </file>
@@ -752,8 +756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1128,26 +1132,26 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" ht="75">
       <c r="A36" t="s">
         <v>57</v>
       </c>
       <c r="C36" t="s">
         <v>10</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>58</v>
+      <c r="D36" s="4" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
+        <v>58</v>
+      </c>
+      <c r="C37" t="s">
         <v>59</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D37" t="s">
         <v>60</v>
-      </c>
-      <c r="D37" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1161,8 +1165,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView topLeftCell="D21" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1250,13 +1254,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -1264,13 +1268,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -1278,13 +1282,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -1315,7 +1319,7 @@
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1329,7 +1333,7 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1343,7 +1347,7 @@
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1371,7 +1375,7 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1511,7 +1515,7 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B32" t="s">
         <v>49</v>
@@ -1550,7 +1554,7 @@
         <v>43</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:4">
@@ -1575,18 +1579,18 @@
         <v>10</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" t="s">
+        <v>58</v>
+      </c>
+      <c r="C40" t="s">
         <v>59</v>
       </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>60</v>
-      </c>
-      <c r="D40" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>